<commit_message>
Adding registration data excel
</commit_message>
<xml_diff>
--- a/src/main/resources/registration-data.xlsx
+++ b/src/main/resources/registration-data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5325ecdb3210e6c8/Wallethub/Test Data/Registration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Coding\Java\Projects\mav_learn\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_AE891744112109510FF7F4BB408609D1D9CF742F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F1802FC-DA6D-41B6-BDB8-549C7326B8FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7309A81D-1B79-44A9-9861-80A892504C09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4530" uniqueCount="3002">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4529" uniqueCount="3002">
   <si>
     <t>Record Number</t>
   </si>
@@ -11593,8 +11593,8 @@
   <dimension ref="A1:BC628"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13885,9 +13885,6 @@
       </c>
       <c r="D93" t="s">
         <v>2139</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>429</v>

</xml_diff>